<commit_message>
Third Commit updated msedge drive
</commit_message>
<xml_diff>
--- a/FindHospital/Driver/iosheets.xlsx
+++ b/FindHospital/Driver/iosheets.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="155">
   <si>
     <t>Hospital</t>
   </si>
@@ -277,6 +277,216 @@
   </si>
   <si>
     <t>Ovum Birthing Center</t>
+  </si>
+  <si>
+    <t>Regal Hospital</t>
+  </si>
+  <si>
+    <t>SMILES Institute of Gastroenterology</t>
+  </si>
+  <si>
+    <t>Ayaansh Hospital</t>
+  </si>
+  <si>
+    <t>North Bangalore Hospital</t>
+  </si>
+  <si>
+    <t>Cytecare Cancer Hospitals</t>
+  </si>
+  <si>
+    <t>Apollo Cradle</t>
+  </si>
+  <si>
+    <t>Altius Hospitals</t>
+  </si>
+  <si>
+    <t>PM Santosha Multi Speciality Hospital</t>
+  </si>
+  <si>
+    <t>Vijayanagar Hospital</t>
+  </si>
+  <si>
+    <t>Kangaroo Care Women &amp; Children Hospital</t>
+  </si>
+  <si>
+    <t>MS Ramaiah Memorial Hospital</t>
+  </si>
+  <si>
+    <t>Rajshekar Hospital</t>
+  </si>
+  <si>
+    <t>Bharath Nursing Home</t>
+  </si>
+  <si>
+    <t>Ramakrishna Smart Hospitals</t>
+  </si>
+  <si>
+    <t>Excel Care Hospital</t>
+  </si>
+  <si>
+    <t>Lotus Multispeciality Center</t>
+  </si>
+  <si>
+    <t>Shishuka Children's Specialty Hospital</t>
+  </si>
+  <si>
+    <t>Icon Hospital Maternity &amp; Multispeciality Centre</t>
+  </si>
+  <si>
+    <t>Panacea Hospital - Nagarabhavi</t>
+  </si>
+  <si>
+    <t>People Tree Maarga</t>
+  </si>
+  <si>
+    <t>Aaxis Hospitals - Powered by Medisync</t>
+  </si>
+  <si>
+    <t>RITU Multispeciality Hospital</t>
+  </si>
+  <si>
+    <t>BMS Hospital</t>
+  </si>
+  <si>
+    <t>K.C. Raju Multi Speciality Hospital</t>
+  </si>
+  <si>
+    <t>Comfort Multispeciality Hospital</t>
+  </si>
+  <si>
+    <t>Suraksha Multi Speciality Hospital</t>
+  </si>
+  <si>
+    <t>Promed Hospital</t>
+  </si>
+  <si>
+    <t>Seventh Day Adventist Hospital</t>
+  </si>
+  <si>
+    <t>Sri Sai Nothside Hospital</t>
+  </si>
+  <si>
+    <t>Sri Sai Krupa Hospital</t>
+  </si>
+  <si>
+    <t>Deeksha Hospital</t>
+  </si>
+  <si>
+    <t>Rajashri Grandhim Speciality Hospital</t>
+  </si>
+  <si>
+    <t>Vijayashree Multi Specialty Hospital</t>
+  </si>
+  <si>
+    <t>Asha Nursing Home</t>
+  </si>
+  <si>
+    <t>Sevakshetra Hospital</t>
+  </si>
+  <si>
+    <t>Geetha Hospital</t>
+  </si>
+  <si>
+    <t>Rajalakshmi Multispeciality Hospital.</t>
+  </si>
+  <si>
+    <t>Sri Devi Hospital</t>
+  </si>
+  <si>
+    <t>Avhieta Health Care and Hospital</t>
+  </si>
+  <si>
+    <t>First Eat Right Clinic</t>
+  </si>
+  <si>
+    <t>Kanva Diagnostic Services Pvt Ltd</t>
+  </si>
+  <si>
+    <t>Apollo Medical Centre</t>
+  </si>
+  <si>
+    <t>First Eat Right Clinic- Jayanagar 4 Block</t>
+  </si>
+  <si>
+    <t>First Eat Right Clinic - Koramangala</t>
+  </si>
+  <si>
+    <t>Chirag Hospital</t>
+  </si>
+  <si>
+    <t>Aster CMI Hospital</t>
+  </si>
+  <si>
+    <t>The Eye Foundation Super Specialty Eye Hospital</t>
+  </si>
+  <si>
+    <t>Milann IVF</t>
+  </si>
+  <si>
+    <t>Manipal Hospital Malleshwaram</t>
+  </si>
+  <si>
+    <t>Primecare Hospital</t>
+  </si>
+  <si>
+    <t>Astra Superspeciality Hospital</t>
+  </si>
+  <si>
+    <t>Anjani Women's Day Care Hospital</t>
+  </si>
+  <si>
+    <t>Royal Bangalore Hospital</t>
+  </si>
+  <si>
+    <t>AyurHealing Ayurveda and Siddha Hospital</t>
+  </si>
+  <si>
+    <t>GVG Invivo Hospitals</t>
+  </si>
+  <si>
+    <t>Tatkshana Ayurveda Hospital</t>
+  </si>
+  <si>
+    <t>N.D.R Medical Centre</t>
+  </si>
+  <si>
+    <t>Jas Dental</t>
+  </si>
+  <si>
+    <t>Narayana Nethralaya</t>
+  </si>
+  <si>
+    <t>Cavalier Hospital</t>
+  </si>
+  <si>
+    <t>People Tree Hospitals</t>
+  </si>
+  <si>
+    <t>The Bangalore Hospital</t>
+  </si>
+  <si>
+    <t>Chris Super Specialty Hospital</t>
+  </si>
+  <si>
+    <t>Apollo Hospital</t>
+  </si>
+  <si>
+    <t>Lakshmi Maternity &amp; Surgical Centre</t>
+  </si>
+  <si>
+    <t>Dr Rudrappas Hospital</t>
+  </si>
+  <si>
+    <t>Healing Earth Multi-Speciality Ayurveda Hospital</t>
+  </si>
+  <si>
+    <t>Femiint Health &amp; Fertility</t>
+  </si>
+  <si>
+    <t>Bangaluru Neuro Centre</t>
+  </si>
+  <si>
+    <t>Sita Bhateja Specialty Hospital</t>
   </si>
 </sst>
 </file>
@@ -656,7 +866,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A78"/>
+  <dimension ref="A1:A126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -994,52 +1204,52 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77">
@@ -1049,7 +1259,247 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>